<commit_message>
Eleventh Commit: completed the triangle test plan file.
</commit_message>
<xml_diff>
--- a/tests/test_plan_triangle.xlsx
+++ b/tests/test_plan_triangle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Intermediate Software Development0315\8. Activities\Module_02\given_files\activity_2\activity_2\tests\shape\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intermediate_software_development\activities\activity_2\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82F31A6-8AFA-4B46-AE54-0E71FA70719A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B5ED24-F960-423A-B944-A5541FF18ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-28920" yWindow="825" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -249,6 +249,61 @@
   </si>
   <si>
     <t>calculate_perimeter</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Attributes Set</t>
+  </si>
+  <si>
+    <t>color: ""
+side_1 : 5
+side_2 : 5
+side_3 : 7</t>
+  </si>
+  <si>
+    <t>color: "blue"
+side_1 : 5
+side_2 : 5
+side_3 : 7</t>
+  </si>
+  <si>
+    <t>ValueError</t>
+  </si>
+  <si>
+    <t>color : "blue"
+side_1 : "5"
+side_2 : 5
+side_3 : 7</t>
+  </si>
+  <si>
+    <t>color : "blue"
+side_1 : 5
+side_2 : "5"
+side_3 : 7</t>
+  </si>
+  <si>
+    <t>color : "blue"
+side_1 : 5
+side_2 : 5
+side_3 : "7"</t>
+  </si>
+  <si>
+    <t>Triangle("blue", 5, 5, 7)</t>
+  </si>
+  <si>
+    <t>Calculated Area</t>
+  </si>
+  <si>
+    <t>Calculated Perimeter</t>
+  </si>
+  <si>
+    <t>The shape color is blue.
+This triangle has three sides with lengths of 5, 5, 7 centimeters.</t>
+  </si>
+  <si>
+    <t>Michael obikwere</t>
   </si>
 </sst>
 </file>
@@ -1109,22 +1164,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" customWidth="1"/>
+    <col min="7" max="7" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:7" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="1.8">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -1136,14 +1191,16 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>34</v>
+      </c>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1152,10 +1209,10 @@
       </c>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
@@ -1175,7 +1232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="11">
         <v>1</v>
@@ -1186,11 +1243,17 @@
       <c r="D7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="12">
         <v>2</v>
@@ -1201,11 +1264,17 @@
       <c r="D8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="12">
         <v>3</v>
@@ -1216,11 +1285,17 @@
       <c r="D9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="11">
         <v>4</v>
@@ -1232,10 +1307,14 @@
         <v>15</v>
       </c>
       <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
         <v>5</v>
       </c>
@@ -1246,10 +1325,14 @@
         <v>16</v>
       </c>
       <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="12">
         <v>6</v>
       </c>
@@ -1259,11 +1342,17 @@
       <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="11">
         <v>7</v>
       </c>
@@ -1273,11 +1362,17 @@
       <c r="D13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11">
         <v>8</v>
       </c>
@@ -1287,11 +1382,17 @@
       <c r="D14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="12">
         <v>9</v>
       </c>
@@ -1301,7 +1402,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="12">
         <v>10</v>
       </c>
@@ -1311,7 +1412,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="11">
         <v>11</v>
       </c>
@@ -1321,7 +1422,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="12">
         <v>12</v>
       </c>
@@ -1331,7 +1432,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="12">
         <v>13</v>
       </c>
@@ -1341,7 +1442,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="11">
         <v>14</v>
       </c>
@@ -1351,7 +1452,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="11">
         <v>15</v>
       </c>
@@ -1361,7 +1462,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="12">
         <v>16</v>
       </c>
@@ -1371,7 +1472,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="12">
         <v>17</v>
       </c>
@@ -1381,7 +1482,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="11">
         <v>18</v>
       </c>
@@ -1391,7 +1492,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="19" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Twelveth Commit, Fix, Feat: Added and ran unittest for the triangle file, corrected a mistake in my calcu area method, and added more detials to my test plan.
</commit_message>
<xml_diff>
--- a/tests/test_plan_triangle.xlsx
+++ b/tests/test_plan_triangle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intermediate_software_development\activities\activity_2\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B5ED24-F960-423A-B944-A5541FF18ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61EEA814-C364-4C09-85F6-1251FAAFB17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="825" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -293,17 +293,19 @@
     <t>Triangle("blue", 5, 5, 7)</t>
   </si>
   <si>
-    <t>Calculated Area</t>
-  </si>
-  <si>
-    <t>Calculated Perimeter</t>
-  </si>
-  <si>
     <t>The shape color is blue.
 This triangle has three sides with lengths of 5, 5, 7 centimeters.</t>
   </si>
   <si>
     <t>Michael obikwere</t>
+  </si>
+  <si>
+    <t>Calculated Perimeter
+17</t>
+  </si>
+  <si>
+    <t>Calculated Area
+12.497499749949988</t>
   </si>
 </sst>
 </file>
@@ -1164,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1196,7 +1198,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3" s="16"/>
     </row>
@@ -1349,7 +1351,7 @@
         <v>22</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1369,7 +1371,7 @@
         <v>22</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1389,7 +1391,7 @@
         <v>22</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Nineteenth Commit: Made some changes to both triangle test plan and test implementation.
</commit_message>
<xml_diff>
--- a/tests/test_plan_triangle.xlsx
+++ b/tests/test_plan_triangle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intermediate_software_development\activities\activity_2\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61EEA814-C364-4C09-85F6-1251FAAFB17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F969224B-B171-4A1A-BBDE-B2F5A89C114F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
@@ -263,49 +263,49 @@
 side_3 : 7</t>
   </si>
   <si>
-    <t>color: "blue"
+    <t>ValueError</t>
+  </si>
+  <si>
+    <t>Michael obikwere</t>
+  </si>
+  <si>
+    <t>Calculated Perimeter
+17</t>
+  </si>
+  <si>
+    <t>Calculated Area
+12.497499749949988</t>
+  </si>
+  <si>
+    <t>color: "Blue"
 side_1 : 5
 side_2 : 5
 side_3 : 7</t>
   </si>
   <si>
-    <t>ValueError</t>
-  </si>
-  <si>
-    <t>color : "blue"
+    <t>color : "Blue"
 side_1 : "5"
 side_2 : 5
 side_3 : 7</t>
   </si>
   <si>
-    <t>color : "blue"
+    <t>color : "Blue"
 side_1 : 5
 side_2 : "5"
 side_3 : 7</t>
   </si>
   <si>
-    <t>color : "blue"
+    <t>color : "Blue"
 side_1 : 5
 side_2 : 5
 side_3 : "7"</t>
   </si>
   <si>
-    <t>Triangle("blue", 5, 5, 7)</t>
-  </si>
-  <si>
-    <t>The shape color is blue.
+    <t>Triangle("Blue", 5, 5, 7)</t>
+  </si>
+  <si>
+    <t>The shape color is Blue.
 This triangle has three sides with lengths of 5, 5, 7 centimeters.</t>
-  </si>
-  <si>
-    <t>Michael obikwere</t>
-  </si>
-  <si>
-    <t>Calculated Perimeter
-17</t>
-  </si>
-  <si>
-    <t>Calculated Area
-12.497499749949988</t>
   </si>
 </sst>
 </file>
@@ -1166,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1198,7 +1198,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D3" s="16"/>
     </row>
@@ -1249,7 +1249,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>23</v>
@@ -1273,7 +1273,7 @@
         <v>24</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1291,10 +1291,10 @@
         <v>22</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1310,10 +1310,10 @@
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.3">
@@ -1328,10 +1328,10 @@
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1345,13 +1345,13 @@
         <v>18</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1365,13 +1365,13 @@
         <v>20</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1385,13 +1385,13 @@
         <v>20</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>22</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>